<commit_message>
updated all canine test cases with function changes
</commit_message>
<xml_diff>
--- a/OutputFiles/TC02_Canine_Filter_Breed-AmerStaffd_Neo4jData.xlsx
+++ b/OutputFiles/TC02_Canine_Filter_Breed-AmerStaffd_Neo4jData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="65">
   <si>
     <t>Case ID</t>
   </si>
@@ -706,26 +706,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
-      </c>
-    </row>
+    <row r="1"/>
     <row r="2">
       <c r="A2" t="s">
         <v>59</v>
@@ -753,7 +734,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -861,51 +842,56 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>